<commit_message>
chore: 新增不需要校验 token API
</commit_message>
<xml_diff>
--- a/public/static/xlsx/用户列表模版.xlsx
+++ b/public/static/xlsx/用户列表模版.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>已有用户账号</t>
   </si>
@@ -49,6 +49,9 @@
     <t>教授</t>
   </si>
   <si>
+    <t>王师傅</t>
+  </si>
+  <si>
     <t>田师傅</t>
   </si>
   <si>
@@ -64,9 +67,18 @@
     <t>C++</t>
   </si>
   <si>
+    <t>php</t>
+  </si>
+  <si>
     <t>students</t>
   </si>
   <si>
+    <t>xxxxx</t>
+  </si>
+  <si>
+    <t>xxxxfadfa</t>
+  </si>
+  <si>
     <t>nihaonihao</t>
   </si>
   <si>
@@ -85,6 +97,9 @@
     <t>大吃货</t>
   </si>
   <si>
+    <t>小吃货</t>
+  </si>
+  <si>
     <t>我的中路特别稳</t>
   </si>
   <si>
@@ -92,6 +107,15 @@
   </si>
   <si>
     <t>wanghaha</t>
+  </si>
+  <si>
+    <t>nihao</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>nihao11</t>
   </si>
 </sst>
 </file>
@@ -468,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J26"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -592,6 +616,46 @@
         <v>26</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>